<commit_message>
First Version Push Button 16x RGB
</commit_message>
<xml_diff>
--- a/Platinen/PushButton_RGB/PushButton_RGB_w_Test_BOM.xlsx
+++ b/Platinen/PushButton_RGB/PushButton_RGB_w_Test_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hardi\Documents\GitHub\MobaLedLib_Docu\Platinen\PushButton_RGB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4DB319-8BEF-48D1-B2A3-AAC6A047C9A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33867D25-1742-4A3F-A4E5-522426FA365F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="2724" windowWidth="17976" windowHeight="10872" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3480" yWindow="3288" windowWidth="14616" windowHeight="11868" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Comment</t>
   </si>
@@ -185,6 +185,15 @@
   </si>
   <si>
     <t>B 470 Ohm</t>
+  </si>
+  <si>
+    <t>LED1</t>
+  </si>
+  <si>
+    <t>0805</t>
+  </si>
+  <si>
+    <t>C2297</t>
   </si>
 </sst>
 </file>
@@ -261,7 +270,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -276,6 +285,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -620,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -774,6 +786,18 @@
         <v>23</v>
       </c>
     </row>
+    <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A11" s="4"/>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>